<commit_message>
150 report without template
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_demo_022-xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_demo_022-xlsx.w3mi.data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
   <si>
     <t>From</t>
   </si>
@@ -207,9 +207,6 @@
     <t>{R-T;cond=sy-tabix;type=integer}</t>
   </si>
   <si>
-    <t>;func= with white font for specific level!</t>
-  </si>
-  <si>
     <t>https://sites.google.com/site/sapxlwb/home/eng/use/examples/ex11a</t>
   </si>
   <si>
@@ -217,6 +214,12 @@
   </si>
   <si>
     <t>https://sites.google.com/site/sapxlwb/home/eng/use/examples/ex12</t>
+  </si>
+  <si>
+    <t>{R-T-CITYFROM;func=FIRST;merge=X}</t>
+  </si>
+  <si>
+    <t>{R-T-CITYTO;func=FIRST;merge=X}</t>
   </si>
 </sst>
 </file>
@@ -349,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -687,21 +690,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -859,7 +853,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1326,7 +1319,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:M1"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1580,11 +1573,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R1" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1595,7 +1588,7 @@
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1629,12 +1622,8 @@
       <c r="K1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="57"/>
-    </row>
-    <row r="2" spans="1:14" ht="33.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1645,7 +1634,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>36</v>
@@ -1669,17 +1658,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="28"/>
+        <v>56</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>17</v>
+      </c>
       <c r="E3" s="28"/>
       <c r="F3" s="33"/>
       <c r="G3" s="33"/>
@@ -1693,14 +1684,8 @@
       <c r="K3" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1723,7 +1708,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1733,12 +1718,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compatibility with ABAP 7.00
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_demo_022-xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_demo_022-xlsx.w3mi.data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MoldaB\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\moldab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -201,9 +201,6 @@
     <t>{R-T-PRICE;func=SUM}</t>
   </si>
   <si>
-    <t>№</t>
-  </si>
-  <si>
     <t>{R-T;cond=sy-tabix;type=integer}</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>{R-T-CITYTO;func=FIRST;merge=X}</t>
+  </si>
+  <si>
+    <t>Pos.</t>
   </si>
 </sst>
 </file>
@@ -1577,7 +1577,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1605,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G1" s="26" t="s">
         <v>4</v>
@@ -1640,7 +1640,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="32" t="s">
         <v>9</v>
@@ -1663,10 +1663,10 @@
         <v>48</v>
       </c>
       <c r="B3" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>56</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>17</v>
@@ -1708,7 +1708,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1718,12 +1718,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merge=X or G* for MS Word
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_demo_022-xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_demo_022-xlsx.w3mi.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modekz\Desktop\Gaziz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76B0ED7-A3C3-40B3-B327-EF5D3408188B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCDC94D-7FFA-42AC-9606-58CAED429D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="5550" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,22 @@
     <definedName name="H_L1_">Sheet2!$H$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="63">
   <si>
     <t>From</t>
   </si>
@@ -215,12 +226,6 @@
     <t>https://sites.google.com/site/sapxlwb/home/eng/use/examples/ex12</t>
   </si>
   <si>
-    <t>{R-T-CITYFROM;func=FIRST;merge=X}</t>
-  </si>
-  <si>
-    <t>{R-T-CITYTO;func=FIRST;merge=X}</t>
-  </si>
-  <si>
     <t>Pos.</t>
   </si>
   <si>
@@ -236,7 +241,41 @@
     <t>{R-T-CONNID;merge=G0}</t>
   </si>
   <si>
-    <t>Make groups like 'G*' to create order based cell merging</t>
+    <t>{R-T-CITYFROM;func=FIRST;merge=G0}</t>
+  </si>
+  <si>
+    <t>{R-T-CITYTO;func=FIRST;merge=G0}</t>
+  </si>
+  <si>
+    <t>The 'merge=X' is greedy &amp; combine all same values to 1 cell</t>
+  </si>
+  <si>
+    <r>
+      <t>On the other hand the 'merge=G*' depends on previous (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) column </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -720,7 +759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -878,6 +917,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1227,21 +1269,21 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="4" width="16.140625" customWidth="1"/>
+    <col min="3" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="7" width="16.140625" customWidth="1"/>
+    <col min="6" max="7" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1260,7 +1302,7 @@
       </c>
       <c r="G2" s="50"/>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="1" customFormat="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1275,7 +1317,7 @@
       </c>
       <c r="G3" s="48"/>
     </row>
-    <row r="4" spans="1:14" ht="22.5" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="22.5" hidden="1" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1350,7 @@
       <c r="M4" s="16"/>
       <c r="N4" s="16"/>
     </row>
-    <row r="5" spans="1:14" ht="11.25" hidden="1" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="11.25" hidden="1" customHeight="1" outlineLevel="2" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1329,7 +1371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1350,7 +1392,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1382,17 +1424,17 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="8" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" customWidth="1"/>
+    <col min="7" max="8" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1403,7 +1445,7 @@
       <c r="L1" s="56"/>
       <c r="M1" s="57"/>
     </row>
-    <row r="2" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
@@ -1426,7 +1468,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" collapsed="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1452,7 +1494,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1478,7 +1520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1502,12 +1544,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1539,21 +1581,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>47</v>
       </c>
@@ -1584,8 +1626,19 @@
       <c r="J1" s="26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="M1" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+    </row>
+    <row r="2" spans="1:21" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>48</v>
       </c>
@@ -1617,12 +1670,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M1:U1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1637,17 +1693,17 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T1" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>47</v>
       </c>
@@ -1679,24 +1735,24 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="33.75" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="E2" s="28" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>60</v>
       </c>
       <c r="F2" s="32" t="s">
         <v>9</v>
@@ -1714,14 +1770,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1734,18 +1790,18 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="4" width="14" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A1" s="40" t="s">
         <v>38</v>
       </c>
@@ -1762,7 +1818,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" s="26" t="s">
         <v>4</v>
@@ -1780,18 +1836,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>36</v>
@@ -1815,15 +1871,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>17</v>
@@ -1842,7 +1898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="40" t="s">
         <v>24</v>
       </c>
@@ -1861,24 +1917,24 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>53</v>
       </c>

</xml_diff>